<commit_message>
Added email system to send attendance to respective teachers
</commit_message>
<xml_diff>
--- a/class_timetable.xlsx
+++ b/class_timetable.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\giris\Desktop\AAS\opencv_attendence\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51F228EC-CAE1-4CE8-AC68-D509368C89B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE28A5C8-C003-418C-8539-B5825DC696EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14616" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>instructor</t>
   </si>
@@ -55,16 +55,36 @@
   </si>
   <si>
     <t>Mr Deepak</t>
+  </si>
+  <si>
+    <t>EVS</t>
+  </si>
+  <si>
+    <t>Mr Tony</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>girishhrudhay@gmail.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -87,14 +107,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -373,15 +396,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>5</v>
       </c>
@@ -394,8 +417,11 @@
       <c r="D1" t="s">
         <v>0</v>
       </c>
+      <c r="E1" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>0.375</v>
       </c>
@@ -409,7 +435,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>0.41666666666666669</v>
       </c>
@@ -423,21 +449,41 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
+        <v>0.75</v>
+      </c>
+      <c r="B4" s="1">
         <v>0.83333333333333337</v>
       </c>
-      <c r="B4" s="1">
+      <c r="C4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" s="1">
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="B5" s="1">
         <v>0.89583333333333337</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C5" t="s">
         <v>8</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D5" t="s">
         <v>9</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E4" r:id="rId1" xr:uid="{1AC6DBA2-CEC4-493B-B7C7-91DEEB304581}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>